<commit_message>
model and trim separated
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -6,7 +6,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Data'!A1:I97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'Data'!A1:J97</definedName>
   </definedNames>
 </workbook>
 </file>
@@ -400,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,21 +416,24 @@
         <v>Model</v>
       </c>
       <c r="D1" t="str">
+        <v>Trim</v>
+      </c>
+      <c r="E1" t="str">
         <v>Ext</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Int</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Acc</v>
       </c>
-      <c r="G1" t="str">
+      <c r="H1" t="str">
         <v>piOs</v>
       </c>
-      <c r="H1" t="str">
+      <c r="I1" t="str">
         <v>Invoice</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>MSRP</v>
       </c>
     </row>
@@ -442,24 +445,27 @@
         <v>2023</v>
       </c>
       <c r="C2" t="str">
-        <v>42452:SPORTAGE X-LINE AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D2" t="str">
+        <v>X-LINE AWD AUTO</v>
+      </c>
+      <c r="E2" t="str">
         <v>KDG: GRAY(KDG)</v>
       </c>
-      <c r="E2" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F2" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G2" t="str">
         <v>015</v>
       </c>
-      <c r="G2" t="str">
+      <c r="H2" t="str">
         <v>CFX CN2 CO CT PR4</v>
       </c>
-      <c r="H2" t="str">
+      <c r="I2" t="str">
         <v>$ 34,003.00</v>
       </c>
-      <c r="I2" t="str">
+      <c r="J2" t="str">
         <v>$ 34,805.00</v>
       </c>
     </row>
@@ -471,24 +477,27 @@
         <v>2023</v>
       </c>
       <c r="C3" t="str">
-        <v>42462:SPORTAGE SX AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D3" t="str">
+        <v>SX AWD AUTO</v>
+      </c>
+      <c r="E3" t="str">
         <v>GWP: WHITE(GWP)</v>
       </c>
-      <c r="E3" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F3" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G3" t="str">
         <v>010</v>
       </c>
-      <c r="G3" t="str">
+      <c r="H3" t="str">
         <v>CA CF CN1 STD</v>
       </c>
-      <c r="H3" t="str">
+      <c r="I3" t="str">
         <v>$ 34,539.00</v>
       </c>
-      <c r="I3" t="str">
+      <c r="J3" t="str">
         <v>$ 35,635.00</v>
       </c>
     </row>
@@ -500,24 +509,27 @@
         <v>2023</v>
       </c>
       <c r="C4" t="str">
-        <v>76472:SORENTO SX 2.5T AWD AUTO</v>
+        <v>SORENTO</v>
       </c>
       <c r="D4" t="str">
+        <v>SX 2.5T AWD AUTO</v>
+      </c>
+      <c r="E4" t="str">
         <v>C7S: GRAY(C7S)</v>
       </c>
-      <c r="E4" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F4" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G4" t="str">
         <v>010</v>
       </c>
-      <c r="G4" t="str">
+      <c r="H4" t="str">
         <v>CF STD</v>
       </c>
-      <c r="H4" t="str">
+      <c r="I4" t="str">
         <v>$ 40,786.00</v>
       </c>
-      <c r="I4" t="str">
+      <c r="J4" t="str">
         <v>$ 42,685.00</v>
       </c>
     </row>
@@ -529,24 +541,27 @@
         <v>2023</v>
       </c>
       <c r="C5" t="str">
-        <v>76482:SORENTO SX-PRESTIGE 2.5T AWD AUTO</v>
+        <v>SORENTO</v>
       </c>
       <c r="D5" t="str">
+        <v>SX-PRESTIGE 2.5T AWD AUTO</v>
+      </c>
+      <c r="E5" t="str">
         <v>GWP: WHITE(GWP)</v>
       </c>
-      <c r="E5" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F5" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G5" t="str">
         <v>010</v>
       </c>
-      <c r="G5" t="str">
+      <c r="H5" t="str">
         <v>CF CN CT STD WL</v>
       </c>
-      <c r="H5" t="str">
+      <c r="I5" t="str">
         <v>$ 44,077.00</v>
       </c>
-      <c r="I5" t="str">
+      <c r="J5" t="str">
         <v>$ 45,720.00</v>
       </c>
     </row>
@@ -558,24 +573,27 @@
         <v>2023</v>
       </c>
       <c r="C6" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D6" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E6" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E6" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F6" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G6" t="str">
         <v>015</v>
       </c>
-      <c r="G6" t="str">
+      <c r="H6" t="str">
         <v>TCC</v>
       </c>
-      <c r="H6" t="str">
+      <c r="I6" t="str">
         <v>$ 21,288.00</v>
       </c>
-      <c r="I6" t="str">
+      <c r="J6" t="str">
         <v>$ 21,815.00</v>
       </c>
     </row>
@@ -587,24 +605,27 @@
         <v>2023</v>
       </c>
       <c r="C7" t="str">
-        <v>C3452:FORTE GT-LINE AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D7" t="str">
+        <v>GT-LINE AUTO</v>
+      </c>
+      <c r="E7" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E7" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F7" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G7" t="str">
         <v>020</v>
       </c>
-      <c r="G7" t="str">
+      <c r="H7" t="str">
         <v>PRC SPC</v>
       </c>
-      <c r="H7" t="str">
+      <c r="I7" t="str">
         <v>$ 25,054.00</v>
       </c>
-      <c r="I7" t="str">
+      <c r="J7" t="str">
         <v>$ 26,010.00</v>
       </c>
     </row>
@@ -616,24 +637,27 @@
         <v>2023</v>
       </c>
       <c r="C8" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D8" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E8" t="str">
         <v>KDG: GRAY(KDG)</v>
       </c>
-      <c r="E8" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F8" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G8" t="str">
         <v>010</v>
       </c>
-      <c r="G8" t="str">
+      <c r="H8" t="str">
         <v>STD</v>
       </c>
-      <c r="H8" t="str">
+      <c r="I8" t="str">
         <v>$ 20,807.00</v>
       </c>
-      <c r="I8" t="str">
+      <c r="J8" t="str">
         <v>$ 21,315.00</v>
       </c>
     </row>
@@ -645,24 +669,27 @@
         <v>2023</v>
       </c>
       <c r="C9" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D9" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E9" t="str">
         <v>KDG: GRAY(KDG)</v>
       </c>
-      <c r="E9" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F9" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G9" t="str">
         <v>015</v>
       </c>
-      <c r="G9" t="str">
+      <c r="H9" t="str">
         <v>TCC</v>
       </c>
-      <c r="H9" t="str">
+      <c r="I9" t="str">
         <v>$ 21,288.00</v>
       </c>
-      <c r="I9" t="str">
+      <c r="J9" t="str">
         <v>$ 21,815.00</v>
       </c>
     </row>
@@ -674,24 +701,27 @@
         <v>2023</v>
       </c>
       <c r="C10" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D10" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E10" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E10" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F10" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G10" t="str">
         <v>015</v>
       </c>
-      <c r="G10" t="str">
+      <c r="H10" t="str">
         <v>TCC</v>
       </c>
-      <c r="H10" t="str">
+      <c r="I10" t="str">
         <v>$ 21,563.00</v>
       </c>
-      <c r="I10" t="str">
+      <c r="J10" t="str">
         <v>$ 22,110.00</v>
       </c>
     </row>
@@ -703,24 +733,27 @@
         <v>2023</v>
       </c>
       <c r="C11" t="str">
-        <v>C3452:FORTE GT-LINE AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D11" t="str">
+        <v>GT-LINE AUTO</v>
+      </c>
+      <c r="E11" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E11" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F11" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G11" t="str">
         <v>020</v>
       </c>
-      <c r="G11" t="str">
+      <c r="H11" t="str">
         <v>PRC SPC</v>
       </c>
-      <c r="H11" t="str">
+      <c r="I11" t="str">
         <v>$ 25,054.00</v>
       </c>
-      <c r="I11" t="str">
+      <c r="J11" t="str">
         <v>$ 26,010.00</v>
       </c>
     </row>
@@ -732,24 +765,27 @@
         <v>2023</v>
       </c>
       <c r="C12" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D12" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E12" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E12" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F12" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G12" t="str">
         <v>010</v>
       </c>
-      <c r="G12" t="str">
+      <c r="H12" t="str">
         <v>STD</v>
       </c>
-      <c r="H12" t="str">
+      <c r="I12" t="str">
         <v>$ 21,083.00</v>
       </c>
-      <c r="I12" t="str">
+      <c r="J12" t="str">
         <v>$ 21,610.00</v>
       </c>
     </row>
@@ -761,24 +797,27 @@
         <v>2023</v>
       </c>
       <c r="C13" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D13" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E13" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E13" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F13" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G13" t="str">
         <v>015</v>
       </c>
-      <c r="G13" t="str">
+      <c r="H13" t="str">
         <v>TCC</v>
       </c>
-      <c r="H13" t="str">
+      <c r="I13" t="str">
         <v>$ 21,288.00</v>
       </c>
-      <c r="I13" t="str">
+      <c r="J13" t="str">
         <v>$ 21,815.00</v>
       </c>
     </row>
@@ -790,24 +829,27 @@
         <v>2023</v>
       </c>
       <c r="C14" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D14" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E14" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E14" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F14" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G14" t="str">
         <v>015</v>
       </c>
-      <c r="G14" t="str">
+      <c r="H14" t="str">
         <v>TCC</v>
       </c>
-      <c r="H14" t="str">
+      <c r="I14" t="str">
         <v>$ 21,563.00</v>
       </c>
-      <c r="I14" t="str">
+      <c r="J14" t="str">
         <v>$ 22,110.00</v>
       </c>
     </row>
@@ -819,24 +861,27 @@
         <v>2023</v>
       </c>
       <c r="C15" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D15" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E15" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E15" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F15" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G15" t="str">
         <v>015</v>
       </c>
-      <c r="G15" t="str">
+      <c r="H15" t="str">
         <v>TCC</v>
       </c>
-      <c r="H15" t="str">
+      <c r="I15" t="str">
         <v>$ 21,563.00</v>
       </c>
-      <c r="I15" t="str">
+      <c r="J15" t="str">
         <v>$ 22,110.00</v>
       </c>
     </row>
@@ -848,24 +893,27 @@
         <v>2023</v>
       </c>
       <c r="C16" t="str">
-        <v>C3422:FORTE LXS AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D16" t="str">
+        <v>LXS AUTO</v>
+      </c>
+      <c r="E16" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E16" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F16" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G16" t="str">
         <v>015</v>
       </c>
-      <c r="G16" t="str">
+      <c r="H16" t="str">
         <v>TCC</v>
       </c>
-      <c r="H16" t="str">
+      <c r="I16" t="str">
         <v>$ 21,563.00</v>
       </c>
-      <c r="I16" t="str">
+      <c r="J16" t="str">
         <v>$ 22,110.00</v>
       </c>
     </row>
@@ -877,24 +925,27 @@
         <v>2023</v>
       </c>
       <c r="C17" t="str">
-        <v>C6482:FORTE GT AUTO</v>
+        <v>FORTE</v>
       </c>
       <c r="D17" t="str">
+        <v>GT AUTO</v>
+      </c>
+      <c r="E17" t="str">
         <v>R4R: RED(R4R)</v>
       </c>
-      <c r="E17" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F17" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G17" t="str">
         <v>015</v>
       </c>
-      <c r="G17" t="str">
+      <c r="H17" t="str">
         <v>G2C</v>
       </c>
-      <c r="H17" t="str">
+      <c r="I17" t="str">
         <v>$ 26,715.00</v>
       </c>
-      <c r="I17" t="str">
+      <c r="J17" t="str">
         <v>$ 27,710.00</v>
       </c>
     </row>
@@ -906,24 +957,27 @@
         <v>2023</v>
       </c>
       <c r="C18" t="str">
-        <v>G4252:NIRO EX TOURING 4CYL AUTO</v>
+        <v>NIRO</v>
       </c>
       <c r="D18" t="str">
+        <v>EX TOURING 4CYL AUTO</v>
+      </c>
+      <c r="E18" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E18" t="str">
+      <c r="F18" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F18" t="str">
+      <c r="G18" t="str">
         <v>015</v>
       </c>
-      <c r="G18" t="str">
+      <c r="H18" t="str">
         <v>CF LBG</v>
       </c>
-      <c r="H18" t="str">
+      <c r="I18" t="str">
         <v>$ 33,070.00</v>
       </c>
-      <c r="I18" t="str">
+      <c r="J18" t="str">
         <v>$ 33,445.00</v>
       </c>
     </row>
@@ -935,24 +989,27 @@
         <v>2023</v>
       </c>
       <c r="C19" t="str">
-        <v>G4242:NIRO EX 4CYL AUTO</v>
+        <v>NIRO</v>
       </c>
       <c r="D19" t="str">
+        <v>EX 4CYL AUTO</v>
+      </c>
+      <c r="E19" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E19" t="str">
+      <c r="F19" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F19" t="str">
+      <c r="G19" t="str">
         <v>015</v>
       </c>
-      <c r="G19" t="str">
+      <c r="H19" t="str">
         <v>CAA CF LBG</v>
       </c>
-      <c r="H19" t="str">
+      <c r="I19" t="str">
         <v>$ 30,503.00</v>
       </c>
-      <c r="I19" t="str">
+      <c r="J19" t="str">
         <v>$ 30,845.00</v>
       </c>
     </row>
@@ -964,24 +1021,27 @@
         <v>2023</v>
       </c>
       <c r="C20" t="str">
-        <v>J4262:TELLURIDE SX V6 FWD AUTO</v>
+        <v>TELLURIDE</v>
       </c>
       <c r="D20" t="str">
+        <v>SX V6 FWD AUTO</v>
+      </c>
+      <c r="E20" t="str">
         <v>MLB: BLUE(MLB)</v>
       </c>
-      <c r="E20" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F20" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G20" t="str">
         <v>012</v>
       </c>
-      <c r="G20" t="str">
+      <c r="H20" t="str">
         <v>CF CN CTS DKC MAJ</v>
       </c>
-      <c r="H20" t="str">
+      <c r="I20" t="str">
         <v>$ 46,507.00</v>
       </c>
-      <c r="I20" t="str">
+      <c r="J20" t="str">
         <v>$ 48,240.00</v>
       </c>
     </row>
@@ -993,24 +1053,27 @@
         <v>2023</v>
       </c>
       <c r="C21" t="str">
-        <v>J4432:TELLURIDE S V6 AWD AUTO</v>
+        <v>TELLURIDE</v>
       </c>
       <c r="D21" t="str">
+        <v>S V6 AWD AUTO</v>
+      </c>
+      <c r="E21" t="str">
         <v>MLB: BLUE(MLB)</v>
       </c>
-      <c r="E21" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F21" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G21" t="str">
         <v>015</v>
       </c>
-      <c r="G21" t="str">
+      <c r="H21" t="str">
         <v>CB CF CN CTS ROJ</v>
       </c>
-      <c r="H21" t="str">
+      <c r="I21" t="str">
         <v>$ 41,828.00</v>
       </c>
-      <c r="I21" t="str">
+      <c r="J21" t="str">
         <v>$ 43,005.00</v>
       </c>
     </row>
@@ -1022,24 +1085,27 @@
         <v>2023</v>
       </c>
       <c r="C22" t="str">
-        <v>J4452:TELLURIDE EX X-LINE V6 AWD AUTO</v>
+        <v>TELLURIDE</v>
       </c>
       <c r="D22" t="str">
+        <v>EX X-LINE V6 AWD AUTO</v>
+      </c>
+      <c r="E22" t="str">
         <v>C7S: GRAY(C7S)</v>
       </c>
-      <c r="E22" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F22" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G22" t="str">
         <v>012</v>
       </c>
-      <c r="G22" t="str">
+      <c r="H22" t="str">
         <v>CF TRJ</v>
       </c>
-      <c r="H22" t="str">
+      <c r="I22" t="str">
         <v>$ 46,822.00</v>
       </c>
-      <c r="I22" t="str">
+      <c r="J22" t="str">
         <v>$ 48,065.00</v>
       </c>
     </row>
@@ -1051,24 +1117,27 @@
         <v>2023</v>
       </c>
       <c r="C23" t="str">
-        <v>J4452:TELLURIDE EX X-LINE V6 AWD AUTO</v>
+        <v>TELLURIDE</v>
       </c>
       <c r="D23" t="str">
+        <v>EX X-LINE V6 AWD AUTO</v>
+      </c>
+      <c r="E23" t="str">
         <v>GWP: WHITE(GWP)</v>
       </c>
-      <c r="E23" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F23" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G23" t="str">
         <v>012</v>
       </c>
-      <c r="G23" t="str">
+      <c r="H23" t="str">
         <v>CBX CF CO CTS TRJ</v>
       </c>
-      <c r="H23" t="str">
+      <c r="I23" t="str">
         <v>$ 47,362.00</v>
       </c>
-      <c r="I23" t="str">
+      <c r="J23" t="str">
         <v>$ 48,695.00</v>
       </c>
     </row>
@@ -1080,24 +1149,27 @@
         <v>2023</v>
       </c>
       <c r="C24" t="str">
-        <v>M4242:CARNIVAL EX AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D24" t="str">
+        <v>EX AUTO</v>
+      </c>
+      <c r="E24" t="str">
         <v>C4S: SILVER(C4S)</v>
       </c>
-      <c r="E24" t="str">
+      <c r="F24" t="str">
         <v>GYT: GRAY(GYT)</v>
       </c>
-      <c r="F24" t="str">
+      <c r="G24" t="str">
         <v>007</v>
       </c>
-      <c r="G24" t="str">
+      <c r="H24" t="str">
         <v>CA CF8 CN CT DWM MUG WL</v>
       </c>
-      <c r="H24" t="str">
+      <c r="I24" t="str">
         <v>$ 40,023.00</v>
       </c>
-      <c r="I24" t="str">
+      <c r="J24" t="str">
         <v>$ 41,140.00</v>
       </c>
     </row>
@@ -1109,24 +1181,27 @@
         <v>2023</v>
       </c>
       <c r="C25" t="str">
-        <v>M4242:CARNIVAL EX AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D25" t="str">
+        <v>EX AUTO</v>
+      </c>
+      <c r="E25" t="str">
         <v>D2U: BLUE(D2U)</v>
       </c>
-      <c r="E25" t="str">
+      <c r="F25" t="str">
         <v>JY2: BROWN(JY2)</v>
       </c>
-      <c r="F25" t="str">
+      <c r="G25" t="str">
         <v>007</v>
       </c>
-      <c r="G25" t="str">
+      <c r="H25" t="str">
         <v>CF8 CN CT DWM MUG WL</v>
       </c>
-      <c r="H25" t="str">
+      <c r="I25" t="str">
         <v>$ 39,945.00</v>
       </c>
-      <c r="I25" t="str">
+      <c r="J25" t="str">
         <v>$ 41,045.00</v>
       </c>
     </row>
@@ -1138,24 +1213,27 @@
         <v>2023</v>
       </c>
       <c r="C26" t="str">
-        <v>N5472:EV6 GT AWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D26" t="str">
+        <v>GT AWD AUTO</v>
+      </c>
+      <c r="E26" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E26" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F26" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G26" t="str">
         <v>010</v>
       </c>
-      <c r="G26" t="str">
+      <c r="H26" t="str">
         <v>CAB CFG STD</v>
       </c>
-      <c r="H26" t="str">
+      <c r="I26" t="str">
         <v>$ 62,148.00</v>
       </c>
-      <c r="I26" t="str">
+      <c r="J26" t="str">
         <v>$ 63,455.00</v>
       </c>
     </row>
@@ -1167,24 +1245,27 @@
         <v>2023</v>
       </c>
       <c r="C27" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D27" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E27" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E27" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F27" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G27" t="str">
         <v>014</v>
       </c>
-      <c r="G27" t="str">
+      <c r="H27" t="str">
         <v>CF CN CO CTL IL ISN SPL</v>
       </c>
-      <c r="H27" t="str">
+      <c r="I27" t="str">
         <v>$ 54,638.00</v>
       </c>
-      <c r="I27" t="str">
+      <c r="J27" t="str">
         <v>$ 55,920.00</v>
       </c>
     </row>
@@ -1196,24 +1277,27 @@
         <v>2023</v>
       </c>
       <c r="C28" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D28" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E28" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E28" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F28" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G28" t="str">
         <v>015</v>
       </c>
-      <c r="G28" t="str">
+      <c r="H28" t="str">
         <v>CF CTL TEN</v>
       </c>
-      <c r="H28" t="str">
+      <c r="I28" t="str">
         <v>$ 51,232.00</v>
       </c>
-      <c r="I28" t="str">
+      <c r="J28" t="str">
         <v>$ 51,815.00</v>
       </c>
     </row>
@@ -1225,24 +1309,27 @@
         <v>2023</v>
       </c>
       <c r="C29" t="str">
-        <v>N5472:EV6 GT AWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D29" t="str">
+        <v>GT AWD AUTO</v>
+      </c>
+      <c r="E29" t="str">
         <v>CR5: RED(CR5)</v>
       </c>
-      <c r="E29" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F29" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G29" t="str">
         <v>010</v>
       </c>
-      <c r="G29" t="str">
+      <c r="H29" t="str">
         <v>CFG CTL STD</v>
       </c>
-      <c r="H29" t="str">
+      <c r="I29" t="str">
         <v>$ 61,937.00</v>
       </c>
-      <c r="I29" t="str">
+      <c r="J29" t="str">
         <v>$ 63,215.00</v>
       </c>
     </row>
@@ -1254,24 +1341,27 @@
         <v>2023</v>
       </c>
       <c r="C30" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D30" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E30" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E30" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F30" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G30" t="str">
         <v>015</v>
       </c>
-      <c r="G30" t="str">
+      <c r="H30" t="str">
         <v>CF CTL TEN</v>
       </c>
-      <c r="H30" t="str">
+      <c r="I30" t="str">
         <v>$ 51,692.00</v>
       </c>
-      <c r="I30" t="str">
+      <c r="J30" t="str">
         <v>$ 52,310.00</v>
       </c>
     </row>
@@ -1283,24 +1373,27 @@
         <v>2023</v>
       </c>
       <c r="C31" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D31" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E31" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E31" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F31" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G31" t="str">
         <v>014</v>
       </c>
-      <c r="G31" t="str">
+      <c r="H31" t="str">
         <v>CF CN ISN</v>
       </c>
-      <c r="H31" t="str">
+      <c r="I31" t="str">
         <v>$ 54,103.00</v>
       </c>
-      <c r="I31" t="str">
+      <c r="J31" t="str">
         <v>$ 55,245.00</v>
       </c>
     </row>
@@ -1312,24 +1405,27 @@
         <v>2023</v>
       </c>
       <c r="C32" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D32" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E32" t="str">
         <v>KLM: MATTE GRAY(KLM)</v>
       </c>
-      <c r="E32" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F32" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G32" t="str">
         <v>014</v>
       </c>
-      <c r="G32" t="str">
+      <c r="H32" t="str">
         <v>CF ISN</v>
       </c>
-      <c r="H32" t="str">
+      <c r="I32" t="str">
         <v>$ 54,243.00</v>
       </c>
-      <c r="I32" t="str">
+      <c r="J32" t="str">
         <v>$ 55,390.00</v>
       </c>
     </row>
@@ -1341,24 +1437,27 @@
         <v>2023</v>
       </c>
       <c r="C33" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D33" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E33" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E33" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F33" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G33" t="str">
         <v>014</v>
       </c>
-      <c r="G33" t="str">
+      <c r="H33" t="str">
         <v>CF CTL ISN</v>
       </c>
-      <c r="H33" t="str">
+      <c r="I33" t="str">
         <v>$ 54,153.00</v>
       </c>
-      <c r="I33" t="str">
+      <c r="J33" t="str">
         <v>$ 55,305.00</v>
       </c>
     </row>
@@ -1370,24 +1469,27 @@
         <v>2023</v>
       </c>
       <c r="C34" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D34" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E34" t="str">
         <v>GLB: OFF-WHITE(GLB)</v>
       </c>
-      <c r="E34" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F34" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G34" t="str">
         <v>015</v>
       </c>
-      <c r="G34" t="str">
+      <c r="H34" t="str">
         <v>CF TEN WL</v>
       </c>
-      <c r="H34" t="str">
+      <c r="I34" t="str">
         <v>$ 51,650.00</v>
       </c>
-      <c r="I34" t="str">
+      <c r="J34" t="str">
         <v>$ 52,260.00</v>
       </c>
     </row>
@@ -1399,24 +1501,27 @@
         <v>2023</v>
       </c>
       <c r="C35" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D35" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E35" t="str">
         <v>AGT: DARK GRAY(AGT)</v>
       </c>
-      <c r="E35" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F35" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G35" t="str">
         <v>010</v>
       </c>
-      <c r="G35" t="str">
+      <c r="H35" t="str">
         <v>CF CO STD</v>
       </c>
-      <c r="H35" t="str">
+      <c r="I35" t="str">
         <v>$ 49,812.00</v>
       </c>
-      <c r="I35" t="str">
+      <c r="J35" t="str">
         <v>$ 50,350.00</v>
       </c>
     </row>
@@ -1428,24 +1533,27 @@
         <v>2023</v>
       </c>
       <c r="C36" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D36" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E36" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E36" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F36" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G36" t="str">
         <v>014</v>
       </c>
-      <c r="G36" t="str">
+      <c r="H36" t="str">
         <v>CF CN ISN</v>
       </c>
-      <c r="H36" t="str">
+      <c r="I36" t="str">
         <v>$ 54,103.00</v>
       </c>
-      <c r="I36" t="str">
+      <c r="J36" t="str">
         <v>$ 55,245.00</v>
       </c>
     </row>
@@ -1457,24 +1565,27 @@
         <v>2023</v>
       </c>
       <c r="C37" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D37" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E37" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E37" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F37" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G37" t="str">
         <v>015</v>
       </c>
-      <c r="G37" t="str">
+      <c r="H37" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H37" t="str">
+      <c r="I37" t="str">
         <v>$ 51,596.00</v>
       </c>
-      <c r="I37" t="str">
+      <c r="J37" t="str">
         <v>$ 52,195.00</v>
       </c>
     </row>
@@ -1486,24 +1597,27 @@
         <v>2023</v>
       </c>
       <c r="C38" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D38" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E38" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E38" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F38" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G38" t="str">
         <v>015</v>
       </c>
-      <c r="G38" t="str">
+      <c r="H38" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H38" t="str">
+      <c r="I38" t="str">
         <v>$ 51,596.00</v>
       </c>
-      <c r="I38" t="str">
+      <c r="J38" t="str">
         <v>$ 52,195.00</v>
       </c>
     </row>
@@ -1515,24 +1629,27 @@
         <v>2023</v>
       </c>
       <c r="C39" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D39" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E39" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E39" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F39" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G39" t="str">
         <v>015</v>
       </c>
-      <c r="G39" t="str">
+      <c r="H39" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H39" t="str">
+      <c r="I39" t="str">
         <v>$ 51,596.00</v>
       </c>
-      <c r="I39" t="str">
+      <c r="J39" t="str">
         <v>$ 52,195.00</v>
       </c>
     </row>
@@ -1544,24 +1661,27 @@
         <v>2023</v>
       </c>
       <c r="C40" t="str">
-        <v>N5452:EV6 WIND AWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D40" t="str">
+        <v>WIND AWD AUTO</v>
+      </c>
+      <c r="E40" t="str">
         <v>B4U: DARK BLUE(B4U)</v>
       </c>
-      <c r="E40" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F40" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G40" t="str">
         <v>010</v>
       </c>
-      <c r="G40" t="str">
+      <c r="H40" t="str">
         <v>CF STD</v>
       </c>
-      <c r="H40" t="str">
+      <c r="I40" t="str">
         <v>$ 53,547.00</v>
       </c>
-      <c r="I40" t="str">
+      <c r="J40" t="str">
         <v>$ 54,100.00</v>
       </c>
     </row>
@@ -1573,24 +1693,27 @@
         <v>2023</v>
       </c>
       <c r="C41" t="str">
-        <v>N5452:EV6 WIND AWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D41" t="str">
+        <v>WIND AWD AUTO</v>
+      </c>
+      <c r="E41" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E41" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F41" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G41" t="str">
         <v>010</v>
       </c>
-      <c r="G41" t="str">
+      <c r="H41" t="str">
         <v>CF STD WL</v>
       </c>
-      <c r="H41" t="str">
+      <c r="I41" t="str">
         <v>$ 54,061.00</v>
       </c>
-      <c r="I41" t="str">
+      <c r="J41" t="str">
         <v>$ 54,660.00</v>
       </c>
     </row>
@@ -1602,24 +1725,27 @@
         <v>2023</v>
       </c>
       <c r="C42" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D42" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E42" t="str">
         <v>DU3: BLUE(DU3)</v>
       </c>
-      <c r="E42" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F42" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G42" t="str">
         <v>015</v>
       </c>
-      <c r="G42" t="str">
+      <c r="H42" t="str">
         <v>CF TEN WL</v>
       </c>
-      <c r="H42" t="str">
+      <c r="I42" t="str">
         <v>$ 51,190.00</v>
       </c>
-      <c r="I42" t="str">
+      <c r="J42" t="str">
         <v>$ 51,765.00</v>
       </c>
     </row>
@@ -1631,24 +1757,27 @@
         <v>2023</v>
       </c>
       <c r="C43" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D43" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E43" t="str">
         <v>B4U: DARK BLUE(B4U)</v>
       </c>
-      <c r="E43" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F43" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G43" t="str">
         <v>010</v>
       </c>
-      <c r="G43" t="str">
+      <c r="H43" t="str">
         <v>CF CO STD WL</v>
       </c>
-      <c r="H43" t="str">
+      <c r="I43" t="str">
         <v>$ 49,866.00</v>
       </c>
-      <c r="I43" t="str">
+      <c r="J43" t="str">
         <v>$ 50,415.00</v>
       </c>
     </row>
@@ -1660,24 +1789,27 @@
         <v>2023</v>
       </c>
       <c r="C44" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D44" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E44" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E44" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F44" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G44" t="str">
         <v>015</v>
       </c>
-      <c r="G44" t="str">
+      <c r="H44" t="str">
         <v>CF CN TEN</v>
       </c>
-      <c r="H44" t="str">
+      <c r="I44" t="str">
         <v>$ 51,642.00</v>
       </c>
-      <c r="I44" t="str">
+      <c r="J44" t="str">
         <v>$ 52,250.00</v>
       </c>
     </row>
@@ -1689,24 +1821,27 @@
         <v>2023</v>
       </c>
       <c r="C45" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D45" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E45" t="str">
         <v>GLB: OFF-WHITE(GLB)</v>
       </c>
-      <c r="E45" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F45" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G45" t="str">
         <v>015</v>
       </c>
-      <c r="G45" t="str">
+      <c r="H45" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H45" t="str">
+      <c r="I45" t="str">
         <v>$ 51,596.00</v>
       </c>
-      <c r="I45" t="str">
+      <c r="J45" t="str">
         <v>$ 52,195.00</v>
       </c>
     </row>
@@ -1718,24 +1853,27 @@
         <v>2023</v>
       </c>
       <c r="C46" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D46" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E46" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E46" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F46" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G46" t="str">
         <v>015</v>
       </c>
-      <c r="G46" t="str">
+      <c r="H46" t="str">
         <v>CF CTL TEN</v>
       </c>
-      <c r="H46" t="str">
+      <c r="I46" t="str">
         <v>$ 51,692.00</v>
       </c>
-      <c r="I46" t="str">
+      <c r="J46" t="str">
         <v>$ 52,310.00</v>
       </c>
     </row>
@@ -1747,24 +1885,27 @@
         <v>2023</v>
       </c>
       <c r="C47" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D47" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E47" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E47" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F47" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G47" t="str">
         <v>015</v>
       </c>
-      <c r="G47" t="str">
+      <c r="H47" t="str">
         <v>CF CN TEN</v>
       </c>
-      <c r="H47" t="str">
+      <c r="I47" t="str">
         <v>$ 51,642.00</v>
       </c>
-      <c r="I47" t="str">
+      <c r="J47" t="str">
         <v>$ 52,250.00</v>
       </c>
     </row>
@@ -1776,24 +1917,27 @@
         <v>2023</v>
       </c>
       <c r="C48" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D48" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E48" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E48" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F48" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G48" t="str">
         <v>015</v>
       </c>
-      <c r="G48" t="str">
+      <c r="H48" t="str">
         <v>CF CO TEN</v>
       </c>
-      <c r="H48" t="str">
+      <c r="I48" t="str">
         <v>$ 51,721.00</v>
       </c>
-      <c r="I48" t="str">
+      <c r="J48" t="str">
         <v>$ 52,345.00</v>
       </c>
     </row>
@@ -1805,24 +1949,27 @@
         <v>2023</v>
       </c>
       <c r="C49" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D49" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E49" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E49" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F49" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G49" t="str">
         <v>015</v>
       </c>
-      <c r="G49" t="str">
+      <c r="H49" t="str">
         <v>CF CN TEN</v>
       </c>
-      <c r="H49" t="str">
+      <c r="I49" t="str">
         <v>$ 51,642.00</v>
       </c>
-      <c r="I49" t="str">
+      <c r="J49" t="str">
         <v>$ 52,250.00</v>
       </c>
     </row>
@@ -1834,24 +1981,27 @@
         <v>2023</v>
       </c>
       <c r="C50" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D50" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E50" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E50" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F50" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G50" t="str">
         <v>014</v>
       </c>
-      <c r="G50" t="str">
+      <c r="H50" t="str">
         <v>CF ISN</v>
       </c>
-      <c r="H50" t="str">
+      <c r="I50" t="str">
         <v>$ 54,057.00</v>
       </c>
-      <c r="I50" t="str">
+      <c r="J50" t="str">
         <v>$ 55,190.00</v>
       </c>
     </row>
@@ -1863,24 +2013,27 @@
         <v>2023</v>
       </c>
       <c r="C51" t="str">
-        <v>N4362:EV6 GT-LINE RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D51" t="str">
+        <v>GT-LINE RWD AUTO</v>
+      </c>
+      <c r="E51" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E51" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F51" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G51" t="str">
         <v>014</v>
       </c>
-      <c r="G51" t="str">
+      <c r="H51" t="str">
         <v>CF ISN</v>
       </c>
-      <c r="H51" t="str">
+      <c r="I51" t="str">
         <v>$ 54,057.00</v>
       </c>
-      <c r="I51" t="str">
+      <c r="J51" t="str">
         <v>$ 55,190.00</v>
       </c>
     </row>
@@ -1892,24 +2045,27 @@
         <v>2023</v>
       </c>
       <c r="C52" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D52" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E52" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E52" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F52" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G52" t="str">
         <v>015</v>
       </c>
-      <c r="G52" t="str">
+      <c r="H52" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H52" t="str">
+      <c r="I52" t="str">
         <v>$ 51,136.00</v>
       </c>
-      <c r="I52" t="str">
+      <c r="J52" t="str">
         <v>$ 51,700.00</v>
       </c>
     </row>
@@ -1921,24 +2077,27 @@
         <v>2023</v>
       </c>
       <c r="C53" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D53" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E53" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E53" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F53" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G53" t="str">
         <v>015</v>
       </c>
-      <c r="G53" t="str">
+      <c r="H53" t="str">
         <v>CF TEN</v>
       </c>
-      <c r="H53" t="str">
+      <c r="I53" t="str">
         <v>$ 51,136.00</v>
       </c>
-      <c r="I53" t="str">
+      <c r="J53" t="str">
         <v>$ 51,700.00</v>
       </c>
     </row>
@@ -1950,24 +2109,27 @@
         <v>2023</v>
       </c>
       <c r="C54" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D54" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E54" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E54" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F54" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G54" t="str">
         <v>010</v>
       </c>
-      <c r="G54" t="str">
+      <c r="H54" t="str">
         <v>CF STD WL</v>
       </c>
-      <c r="H54" t="str">
+      <c r="I54" t="str">
         <v>$ 49,741.00</v>
       </c>
-      <c r="I54" t="str">
+      <c r="J54" t="str">
         <v>$ 50,265.00</v>
       </c>
     </row>
@@ -1979,24 +2141,27 @@
         <v>2023</v>
       </c>
       <c r="C55" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D55" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E55" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E55" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F55" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G55" t="str">
         <v>010</v>
       </c>
-      <c r="G55" t="str">
+      <c r="H55" t="str">
         <v>CF CN STD</v>
       </c>
-      <c r="H55" t="str">
+      <c r="I55" t="str">
         <v>$ 49,733.00</v>
       </c>
-      <c r="I55" t="str">
+      <c r="J55" t="str">
         <v>$ 50,255.00</v>
       </c>
     </row>
@@ -2008,24 +2173,27 @@
         <v>2023</v>
       </c>
       <c r="C56" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D56" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E56" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E56" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F56" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G56" t="str">
         <v>010</v>
       </c>
-      <c r="G56" t="str">
+      <c r="H56" t="str">
         <v>CF CO STD</v>
       </c>
-      <c r="H56" t="str">
+      <c r="I56" t="str">
         <v>$ 49,812.00</v>
       </c>
-      <c r="I56" t="str">
+      <c r="J56" t="str">
         <v>$ 50,350.00</v>
       </c>
     </row>
@@ -2037,24 +2205,27 @@
         <v>2023</v>
       </c>
       <c r="C57" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D57" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E57" t="str">
         <v>CR5: RED(CR5)</v>
       </c>
-      <c r="E57" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F57" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G57" t="str">
         <v>015</v>
       </c>
-      <c r="G57" t="str">
+      <c r="H57" t="str">
         <v>CF CTL TEN</v>
       </c>
-      <c r="H57" t="str">
+      <c r="I57" t="str">
         <v>$ 51,232.00</v>
       </c>
-      <c r="I57" t="str">
+      <c r="J57" t="str">
         <v>$ 51,815.00</v>
       </c>
     </row>
@@ -2066,24 +2237,27 @@
         <v>2023</v>
       </c>
       <c r="C58" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D58" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E58" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E58" t="str">
+      <c r="F58" t="str">
         <v>CVH: GRAY(CVH)</v>
       </c>
-      <c r="F58" t="str">
+      <c r="G58" t="str">
         <v>015</v>
       </c>
-      <c r="G58" t="str">
+      <c r="H58" t="str">
         <v>CF CN TEN</v>
       </c>
-      <c r="H58" t="str">
+      <c r="I58" t="str">
         <v>$ 51,642.00</v>
       </c>
-      <c r="I58" t="str">
+      <c r="J58" t="str">
         <v>$ 52,250.00</v>
       </c>
     </row>
@@ -2095,24 +2269,27 @@
         <v>2023</v>
       </c>
       <c r="C59" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D59" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E59" t="str">
         <v>B4U: DARK BLUE(B4U)</v>
       </c>
-      <c r="E59" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F59" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G59" t="str">
         <v>015</v>
       </c>
-      <c r="G59" t="str">
+      <c r="H59" t="str">
         <v>CF CN TEN</v>
       </c>
-      <c r="H59" t="str">
+      <c r="I59" t="str">
         <v>$ 51,182.00</v>
       </c>
-      <c r="I59" t="str">
+      <c r="J59" t="str">
         <v>$ 51,755.00</v>
       </c>
     </row>
@@ -2124,24 +2301,27 @@
         <v>2023</v>
       </c>
       <c r="C60" t="str">
-        <v>N4352:EV6 WIND RWD AUTO</v>
+        <v>EV6</v>
       </c>
       <c r="D60" t="str">
+        <v>WIND RWD AUTO</v>
+      </c>
+      <c r="E60" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E60" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F60" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G60" t="str">
         <v>015</v>
       </c>
-      <c r="G60" t="str">
+      <c r="H60" t="str">
         <v>CAB CF TEN</v>
       </c>
-      <c r="H60" t="str">
+      <c r="I60" t="str">
         <v>$ 51,674.00</v>
       </c>
-      <c r="I60" t="str">
+      <c r="J60" t="str">
         <v>$ 52,290.00</v>
       </c>
     </row>
@@ -2153,24 +2333,27 @@
         <v>2023</v>
       </c>
       <c r="C61" t="str">
-        <v>S4482:SPORTAGE HYBRID SX-PRESTIGE AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D61" t="str">
+        <v>HYBRID SX-PRESTIGE AWD AUTO</v>
+      </c>
+      <c r="E61" t="str">
         <v>BB2: BLUE(BB2)</v>
       </c>
-      <c r="E61" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F61" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G61" t="str">
         <v>010</v>
       </c>
-      <c r="G61" t="str">
+      <c r="H61" t="str">
         <v>CF EH STD</v>
       </c>
-      <c r="H61" t="str">
+      <c r="I61" t="str">
         <v>$ 37,427.00</v>
       </c>
-      <c r="I61" t="str">
+      <c r="J61" t="str">
         <v>$ 38,240.00</v>
       </c>
     </row>
@@ -2182,24 +2365,27 @@
         <v>2023</v>
       </c>
       <c r="C62" t="str">
-        <v>S4482:SPORTAGE HYBRID SX-PRESTIGE AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D62" t="str">
+        <v>HYBRID SX-PRESTIGE AWD AUTO</v>
+      </c>
+      <c r="E62" t="str">
         <v>MGG: MATTE GRAY(MGG)</v>
       </c>
-      <c r="E62" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F62" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G62" t="str">
         <v>010</v>
       </c>
-      <c r="G62" t="str">
+      <c r="H62" t="str">
         <v>CB CF EH STD</v>
       </c>
-      <c r="H62" t="str">
+      <c r="I62" t="str">
         <v>$ 38,661.00</v>
       </c>
-      <c r="I62" t="str">
+      <c r="J62" t="str">
         <v>$ 39,195.00</v>
       </c>
     </row>
@@ -2211,24 +2397,27 @@
         <v>2023</v>
       </c>
       <c r="C63" t="str">
-        <v>S4482:SPORTAGE HYBRID SX-PRESTIGE AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D63" t="str">
+        <v>HYBRID SX-PRESTIGE AWD AUTO</v>
+      </c>
+      <c r="E63" t="str">
         <v>MGG: MATTE GRAY(MGG)</v>
       </c>
-      <c r="E63" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F63" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G63" t="str">
         <v>012</v>
       </c>
-      <c r="G63" t="str">
+      <c r="H63" t="str">
         <v>CB CF EH RLS</v>
       </c>
-      <c r="H63" t="str">
+      <c r="I63" t="str">
         <v>$ 38,661.00</v>
       </c>
-      <c r="I63" t="str">
+      <c r="J63" t="str">
         <v>$ 39,195.00</v>
       </c>
     </row>
@@ -2240,24 +2429,27 @@
         <v>2023</v>
       </c>
       <c r="C64" t="str">
-        <v>S4422:SPORTAGE HYBRID LX AWD AUTO</v>
+        <v>SPORTAGE</v>
       </c>
       <c r="D64" t="str">
+        <v>HYBRID LX AWD AUTO</v>
+      </c>
+      <c r="E64" t="str">
         <v>FSB: BLACK(FSB)</v>
       </c>
-      <c r="E64" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F64" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G64" t="str">
         <v>010</v>
       </c>
-      <c r="G64" t="str">
+      <c r="H64" t="str">
         <v>CF CN2 STD</v>
       </c>
-      <c r="H64" t="str">
+      <c r="I64" t="str">
         <v>$ 30,511.00</v>
       </c>
-      <c r="I64" t="str">
+      <c r="J64" t="str">
         <v>$ 30,845.00</v>
       </c>
     </row>
@@ -2269,24 +2461,27 @@
         <v>2023</v>
       </c>
       <c r="C65" t="str">
-        <v>U4242:SORENTO HYBRID EX FWD AUTO</v>
+        <v>SORENTO</v>
       </c>
       <c r="D65" t="str">
+        <v>HYBRID EX FWD AUTO</v>
+      </c>
+      <c r="E65" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E65" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F65" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G65" t="str">
         <v>010</v>
       </c>
-      <c r="G65" t="str">
+      <c r="H65" t="str">
         <v>CF CO CTS MUG SS STD WL</v>
       </c>
-      <c r="H65" t="str">
+      <c r="I65" t="str">
         <v>$ 38,638.00</v>
       </c>
-      <c r="I65" t="str">
+      <c r="J65" t="str">
         <v>$ 39,425.00</v>
       </c>
     </row>
@@ -2298,24 +2493,27 @@
         <v>2023</v>
       </c>
       <c r="C66" t="str">
-        <v>U4462:SORENTO HYBRID SX-PRESTIGE AWD AUTO</v>
+        <v>SORENTO</v>
       </c>
       <c r="D66" t="str">
+        <v>HYBRID SX-PRESTIGE AWD AUTO</v>
+      </c>
+      <c r="E66" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E66" t="str">
+      <c r="F66" t="str">
         <v>GYT: GRAY(GYT)</v>
       </c>
-      <c r="F66" t="str">
+      <c r="G66" t="str">
         <v>010</v>
       </c>
-      <c r="G66" t="str">
+      <c r="H66" t="str">
         <v>CF STD</v>
       </c>
-      <c r="H66" t="str">
+      <c r="I66" t="str">
         <v>$ 43,358.00</v>
       </c>
-      <c r="I66" t="str">
+      <c r="J66" t="str">
         <v>$ 44,040.00</v>
       </c>
     </row>
@@ -2327,24 +2525,27 @@
         <v>2023</v>
       </c>
       <c r="C67" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D67" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E67" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E67" t="str">
+      <c r="F67" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F67" t="str">
+      <c r="G67" t="str">
         <v>020</v>
       </c>
-      <c r="G67" t="str">
+      <c r="H67" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H67" t="str">
+      <c r="I67" t="str">
         <v>$ 41,052.00</v>
       </c>
-      <c r="I67" t="str">
+      <c r="J67" t="str">
         <v>$ 41,505.00</v>
       </c>
     </row>
@@ -2356,24 +2557,27 @@
         <v>2023</v>
       </c>
       <c r="C68" t="str">
-        <v>V1282:NIRO EV WAVE</v>
+        <v>NIRO</v>
       </c>
       <c r="D68" t="str">
+        <v>EV WAVE</v>
+      </c>
+      <c r="E68" t="str">
         <v>DRG: ORANGE(DRG)</v>
       </c>
-      <c r="E68" t="str">
+      <c r="F68" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F68" t="str">
+      <c r="G68" t="str">
         <v>020</v>
       </c>
-      <c r="G68" t="str">
+      <c r="H68" t="str">
         <v>CF CTA DKC LBV</v>
       </c>
-      <c r="H68" t="str">
+      <c r="I68" t="str">
         <v>$ 45,286.00</v>
       </c>
-      <c r="I68" t="str">
+      <c r="J68" t="str">
         <v>$ 46,225.00</v>
       </c>
     </row>
@@ -2385,24 +2589,27 @@
         <v>2023</v>
       </c>
       <c r="C69" t="str">
-        <v>V1282:NIRO EV WAVE</v>
+        <v>NIRO</v>
       </c>
       <c r="D69" t="str">
+        <v>EV WAVE</v>
+      </c>
+      <c r="E69" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E69" t="str">
+      <c r="F69" t="str">
         <v>EWR: LT GRAY(EWR)</v>
       </c>
-      <c r="F69" t="str">
+      <c r="G69" t="str">
         <v>022</v>
       </c>
-      <c r="G69" t="str">
+      <c r="H69" t="str">
         <v>CF CTA DKC GCV LBV</v>
       </c>
-      <c r="H69" t="str">
+      <c r="I69" t="str">
         <v>$ 45,286.00</v>
       </c>
-      <c r="I69" t="str">
+      <c r="J69" t="str">
         <v>$ 46,225.00</v>
       </c>
     </row>
@@ -2414,24 +2621,27 @@
         <v>2023</v>
       </c>
       <c r="C70" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D70" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E70" t="str">
         <v>DRG: ORANGE(DRG)</v>
       </c>
-      <c r="E70" t="str">
+      <c r="F70" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F70" t="str">
+      <c r="G70" t="str">
         <v>020</v>
       </c>
-      <c r="G70" t="str">
+      <c r="H70" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H70" t="str">
+      <c r="I70" t="str">
         <v>$ 40,685.00</v>
       </c>
-      <c r="I70" t="str">
+      <c r="J70" t="str">
         <v>$ 41,110.00</v>
       </c>
     </row>
@@ -2443,24 +2653,27 @@
         <v>2023</v>
       </c>
       <c r="C71" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D71" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E71" t="str">
         <v>DRG: ORANGE(DRG)</v>
       </c>
-      <c r="E71" t="str">
+      <c r="F71" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F71" t="str">
+      <c r="G71" t="str">
         <v>020</v>
       </c>
-      <c r="G71" t="str">
+      <c r="H71" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H71" t="str">
+      <c r="I71" t="str">
         <v>$ 40,685.00</v>
       </c>
-      <c r="I71" t="str">
+      <c r="J71" t="str">
         <v>$ 41,110.00</v>
       </c>
     </row>
@@ -2472,24 +2685,27 @@
         <v>2023</v>
       </c>
       <c r="C72" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D72" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E72" t="str">
         <v>DRG: ORANGE(DRG)</v>
       </c>
-      <c r="E72" t="str">
+      <c r="F72" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F72" t="str">
+      <c r="G72" t="str">
         <v>020</v>
       </c>
-      <c r="G72" t="str">
+      <c r="H72" t="str">
         <v>CF CTA LBV</v>
       </c>
-      <c r="H72" t="str">
+      <c r="I72" t="str">
         <v>$ 40,781.00</v>
       </c>
-      <c r="I72" t="str">
+      <c r="J72" t="str">
         <v>$ 41,225.00</v>
       </c>
     </row>
@@ -2501,24 +2717,27 @@
         <v>2023</v>
       </c>
       <c r="C73" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D73" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E73" t="str">
         <v>CGE: GREEN(CGE)</v>
       </c>
-      <c r="E73" t="str">
+      <c r="F73" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F73" t="str">
+      <c r="G73" t="str">
         <v>020</v>
       </c>
-      <c r="G73" t="str">
+      <c r="H73" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H73" t="str">
+      <c r="I73" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I73" t="str">
+      <c r="J73" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2530,24 +2749,27 @@
         <v>2023</v>
       </c>
       <c r="C74" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D74" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E74" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E74" t="str">
+      <c r="F74" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F74" t="str">
+      <c r="G74" t="str">
         <v>020</v>
       </c>
-      <c r="G74" t="str">
+      <c r="H74" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H74" t="str">
+      <c r="I74" t="str">
         <v>$ 41,052.00</v>
       </c>
-      <c r="I74" t="str">
+      <c r="J74" t="str">
         <v>$ 41,505.00</v>
       </c>
     </row>
@@ -2559,24 +2781,27 @@
         <v>2023</v>
       </c>
       <c r="C75" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D75" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E75" t="str">
         <v>CGE: GREEN(CGE)</v>
       </c>
-      <c r="E75" t="str">
+      <c r="F75" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F75" t="str">
+      <c r="G75" t="str">
         <v>020</v>
       </c>
-      <c r="G75" t="str">
+      <c r="H75" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H75" t="str">
+      <c r="I75" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I75" t="str">
+      <c r="J75" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2588,24 +2813,27 @@
         <v>2023</v>
       </c>
       <c r="C76" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D76" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E76" t="str">
         <v>CGE: GREEN(CGE)</v>
       </c>
-      <c r="E76" t="str">
+      <c r="F76" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F76" t="str">
+      <c r="G76" t="str">
         <v>020</v>
       </c>
-      <c r="G76" t="str">
+      <c r="H76" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H76" t="str">
+      <c r="I76" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I76" t="str">
+      <c r="J76" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2617,24 +2845,27 @@
         <v>2023</v>
       </c>
       <c r="C77" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D77" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E77" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E77" t="str">
+      <c r="F77" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F77" t="str">
+      <c r="G77" t="str">
         <v>020</v>
       </c>
-      <c r="G77" t="str">
+      <c r="H77" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H77" t="str">
+      <c r="I77" t="str">
         <v>$ 41,052.00</v>
       </c>
-      <c r="I77" t="str">
+      <c r="J77" t="str">
         <v>$ 41,505.00</v>
       </c>
     </row>
@@ -2646,24 +2877,27 @@
         <v>2023</v>
       </c>
       <c r="C78" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D78" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E78" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E78" t="str">
+      <c r="F78" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F78" t="str">
+      <c r="G78" t="str">
         <v>020</v>
       </c>
-      <c r="G78" t="str">
+      <c r="H78" t="str">
         <v>CF LBV</v>
       </c>
-      <c r="H78" t="str">
+      <c r="I78" t="str">
         <v>$ 41,052.00</v>
       </c>
-      <c r="I78" t="str">
+      <c r="J78" t="str">
         <v>$ 41,505.00</v>
       </c>
     </row>
@@ -2675,24 +2909,27 @@
         <v>2023</v>
       </c>
       <c r="C79" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D79" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E79" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E79" t="str">
+      <c r="F79" t="str">
         <v>EWR: LT GRAY(EWR)</v>
       </c>
-      <c r="F79" t="str">
+      <c r="G79" t="str">
         <v>022</v>
       </c>
-      <c r="G79" t="str">
+      <c r="H79" t="str">
         <v>CF GCV LBV WL</v>
       </c>
-      <c r="H79" t="str">
+      <c r="I79" t="str">
         <v>$ 41,106.00</v>
       </c>
-      <c r="I79" t="str">
+      <c r="J79" t="str">
         <v>$ 41,570.00</v>
       </c>
     </row>
@@ -2704,24 +2941,27 @@
         <v>2023</v>
       </c>
       <c r="C80" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D80" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E80" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E80" t="str">
+      <c r="F80" t="str">
         <v>EWR: LT GRAY(EWR)</v>
       </c>
-      <c r="F80" t="str">
+      <c r="G80" t="str">
         <v>022</v>
       </c>
-      <c r="G80" t="str">
+      <c r="H80" t="str">
         <v>CF GCV LBV</v>
       </c>
-      <c r="H80" t="str">
+      <c r="I80" t="str">
         <v>$ 40,685.00</v>
       </c>
-      <c r="I80" t="str">
+      <c r="J80" t="str">
         <v>$ 41,110.00</v>
       </c>
     </row>
@@ -2733,24 +2973,27 @@
         <v>2023</v>
       </c>
       <c r="C81" t="str">
-        <v>V1282:NIRO EV WAVE</v>
+        <v>NIRO</v>
       </c>
       <c r="D81" t="str">
+        <v>EV WAVE</v>
+      </c>
+      <c r="E81" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E81" t="str">
+      <c r="F81" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F81" t="str">
+      <c r="G81" t="str">
         <v>020</v>
       </c>
-      <c r="G81" t="str">
+      <c r="H81" t="str">
         <v>CF CTA DKC LBV</v>
       </c>
-      <c r="H81" t="str">
+      <c r="I81" t="str">
         <v>$ 45,653.00</v>
       </c>
-      <c r="I81" t="str">
+      <c r="J81" t="str">
         <v>$ 46,620.00</v>
       </c>
     </row>
@@ -2762,24 +3005,27 @@
         <v>2023</v>
       </c>
       <c r="C82" t="str">
-        <v>V1282:NIRO EV WAVE</v>
+        <v>NIRO</v>
       </c>
       <c r="D82" t="str">
+        <v>EV WAVE</v>
+      </c>
+      <c r="E82" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E82" t="str">
+      <c r="F82" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F82" t="str">
+      <c r="G82" t="str">
         <v>020</v>
       </c>
-      <c r="G82" t="str">
+      <c r="H82" t="str">
         <v>DKC LBV</v>
       </c>
-      <c r="H82" t="str">
+      <c r="I82" t="str">
         <v>$ 45,412.00</v>
       </c>
-      <c r="I82" t="str">
+      <c r="J82" t="str">
         <v>$ 46,330.00</v>
       </c>
     </row>
@@ -2791,24 +3037,27 @@
         <v>2023</v>
       </c>
       <c r="C83" t="str">
-        <v>V1282:NIRO EV WAVE</v>
+        <v>NIRO</v>
       </c>
       <c r="D83" t="str">
+        <v>EV WAVE</v>
+      </c>
+      <c r="E83" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E83" t="str">
+      <c r="F83" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F83" t="str">
+      <c r="G83" t="str">
         <v>020</v>
       </c>
-      <c r="G83" t="str">
+      <c r="H83" t="str">
         <v>CF CN CTA DKC LBV</v>
       </c>
-      <c r="H83" t="str">
+      <c r="I83" t="str">
         <v>$ 45,332.00</v>
       </c>
-      <c r="I83" t="str">
+      <c r="J83" t="str">
         <v>$ 46,280.00</v>
       </c>
     </row>
@@ -2820,24 +3069,27 @@
         <v>2023</v>
       </c>
       <c r="C84" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D84" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E84" t="str">
         <v>AGT: GRAY(AGT)</v>
       </c>
-      <c r="E84" t="str">
+      <c r="F84" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F84" t="str">
+      <c r="G84" t="str">
         <v>020</v>
       </c>
-      <c r="G84" t="str">
+      <c r="H84" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H84" t="str">
+      <c r="I84" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I84" t="str">
+      <c r="J84" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2849,24 +3101,27 @@
         <v>2023</v>
       </c>
       <c r="C85" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D85" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E85" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E85" t="str">
+      <c r="F85" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F85" t="str">
+      <c r="G85" t="str">
         <v>020</v>
       </c>
-      <c r="G85" t="str">
+      <c r="H85" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H85" t="str">
+      <c r="I85" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I85" t="str">
+      <c r="J85" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2878,24 +3133,27 @@
         <v>2023</v>
       </c>
       <c r="C86" t="str">
-        <v>V1242:NIRO EV WIND</v>
+        <v>NIRO</v>
       </c>
       <c r="D86" t="str">
+        <v>EV WIND</v>
+      </c>
+      <c r="E86" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E86" t="str">
+      <c r="F86" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F86" t="str">
+      <c r="G86" t="str">
         <v>020</v>
       </c>
-      <c r="G86" t="str">
+      <c r="H86" t="str">
         <v>CF CN LBV</v>
       </c>
-      <c r="H86" t="str">
+      <c r="I86" t="str">
         <v>$ 40,731.00</v>
       </c>
-      <c r="I86" t="str">
+      <c r="J86" t="str">
         <v>$ 41,165.00</v>
       </c>
     </row>
@@ -2907,24 +3165,27 @@
         <v>2023</v>
       </c>
       <c r="C87" t="str">
-        <v>W4242:NIRO PHEV EX</v>
+        <v>NIRO</v>
       </c>
       <c r="D87" t="str">
+        <v>PHEV EX</v>
+      </c>
+      <c r="E87" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E87" t="str">
+      <c r="F87" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F87" t="str">
+      <c r="G87" t="str">
         <v>010</v>
       </c>
-      <c r="G87" t="str">
+      <c r="H87" t="str">
         <v>CA CF IL MUG STD</v>
       </c>
-      <c r="H87" t="str">
+      <c r="I87" t="str">
         <v>$ 35,277.00</v>
       </c>
-      <c r="I87" t="str">
+      <c r="J87" t="str">
         <v>$ 35,725.00</v>
       </c>
     </row>
@@ -2936,24 +3197,27 @@
         <v>2023</v>
       </c>
       <c r="C88" t="str">
-        <v>W4242:NIRO PHEV EX</v>
+        <v>NIRO</v>
       </c>
       <c r="D88" t="str">
+        <v>PHEV EX</v>
+      </c>
+      <c r="E88" t="str">
         <v>CGE: GREEN(CGE)</v>
       </c>
-      <c r="E88" t="str">
+      <c r="F88" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F88" t="str">
+      <c r="G88" t="str">
         <v>010</v>
       </c>
-      <c r="G88" t="str">
+      <c r="H88" t="str">
         <v>CF STD</v>
       </c>
-      <c r="H88" t="str">
+      <c r="I88" t="str">
         <v>$ 34,969.00</v>
       </c>
-      <c r="I88" t="str">
+      <c r="J88" t="str">
         <v>$ 35,340.00</v>
       </c>
     </row>
@@ -2965,24 +3229,27 @@
         <v>2023</v>
       </c>
       <c r="C89" t="str">
-        <v>W4242:NIRO PHEV EX</v>
+        <v>NIRO</v>
       </c>
       <c r="D89" t="str">
+        <v>PHEV EX</v>
+      </c>
+      <c r="E89" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E89" t="str">
+      <c r="F89" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F89" t="str">
+      <c r="G89" t="str">
         <v>015</v>
       </c>
-      <c r="G89" t="str">
+      <c r="H89" t="str">
         <v>CF PEW</v>
       </c>
-      <c r="H89" t="str">
+      <c r="I89" t="str">
         <v>$ 35,918.00</v>
       </c>
-      <c r="I89" t="str">
+      <c r="J89" t="str">
         <v>$ 36,335.00</v>
       </c>
     </row>
@@ -2994,24 +3261,27 @@
         <v>2023</v>
       </c>
       <c r="C90" t="str">
-        <v>W4242:NIRO PHEV EX</v>
+        <v>NIRO</v>
       </c>
       <c r="D90" t="str">
+        <v>PHEV EX</v>
+      </c>
+      <c r="E90" t="str">
         <v>M4B: BLUE(M4B)</v>
       </c>
-      <c r="E90" t="str">
+      <c r="F90" t="str">
         <v>CCV: DK GRAY(CCV)</v>
       </c>
-      <c r="F90" t="str">
+      <c r="G90" t="str">
         <v>010</v>
       </c>
-      <c r="G90" t="str">
+      <c r="H90" t="str">
         <v>CF CN CT STD WL</v>
       </c>
-      <c r="H90" t="str">
+      <c r="I90" t="str">
         <v>$ 35,167.00</v>
       </c>
-      <c r="I90" t="str">
+      <c r="J90" t="str">
         <v>$ 35,575.00</v>
       </c>
     </row>
@@ -3023,24 +3293,27 @@
         <v>2024</v>
       </c>
       <c r="C91" t="str">
-        <v>K2232:SELTOS S FWD AUTO</v>
+        <v>SELTOS</v>
       </c>
       <c r="D91" t="str">
+        <v>S FWD AUTO</v>
+      </c>
+      <c r="E91" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E91" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F91" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G91" t="str">
         <v>014</v>
       </c>
-      <c r="G91" t="str">
+      <c r="H91" t="str">
         <v>CF NVK</v>
       </c>
-      <c r="H91" t="str">
+      <c r="I91" t="str">
         <v>$ 26,202.00</v>
       </c>
-      <c r="I91" t="str">
+      <c r="J91" t="str">
         <v>$ 26,885.00</v>
       </c>
     </row>
@@ -3052,24 +3325,27 @@
         <v>2024</v>
       </c>
       <c r="C92" t="str">
-        <v>K2232:SELTOS S FWD AUTO</v>
+        <v>SELTOS</v>
       </c>
       <c r="D92" t="str">
+        <v>S FWD AUTO</v>
+      </c>
+      <c r="E92" t="str">
         <v>SWP: WHITE(SWP)</v>
       </c>
-      <c r="E92" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F92" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G92" t="str">
         <v>010</v>
       </c>
-      <c r="G92" t="str">
+      <c r="H92" t="str">
         <v>CF STD</v>
       </c>
-      <c r="H92" t="str">
+      <c r="I92" t="str">
         <v>$ 26,202.00</v>
       </c>
-      <c r="I92" t="str">
+      <c r="J92" t="str">
         <v>$ 26,885.00</v>
       </c>
     </row>
@@ -3081,24 +3357,27 @@
         <v>2024</v>
       </c>
       <c r="C93" t="str">
-        <v>K4452:SELTOS X-LINE 1.6T AWD AUTO</v>
+        <v>SELTOS</v>
       </c>
       <c r="D93" t="str">
+        <v>X-LINE 1.6T AWD AUTO</v>
+      </c>
+      <c r="E93" t="str">
         <v>KLG: GRAY(KLG)</v>
       </c>
-      <c r="E93" t="str">
-        <v>WK: BLACK(WK)</v>
-      </c>
       <c r="F93" t="str">
+        <v>WK: BLACK(WK)</v>
+      </c>
+      <c r="G93" t="str">
         <v>010</v>
       </c>
-      <c r="G93" t="str">
+      <c r="H93" t="str">
         <v>CBX CF CTR STD</v>
       </c>
-      <c r="H93" t="str">
+      <c r="I93" t="str">
         <v>$ 29,869.00</v>
       </c>
-      <c r="I93" t="str">
+      <c r="J93" t="str">
         <v>$ 30,690.00</v>
       </c>
     </row>
@@ -3110,24 +3389,27 @@
         <v>2024</v>
       </c>
       <c r="C94" t="str">
-        <v>M4282:CARNIVAL SX AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D94" t="str">
+        <v>SX AUTO</v>
+      </c>
+      <c r="E94" t="str">
         <v>C7R: RED(C7R)</v>
       </c>
-      <c r="E94" t="str">
+      <c r="F94" t="str">
         <v>GYT: GRAY(GYT)</v>
       </c>
-      <c r="F94" t="str">
+      <c r="G94" t="str">
         <v>015</v>
       </c>
-      <c r="G94" t="str">
+      <c r="H94" t="str">
         <v>CA CF8 CN ENM WL</v>
       </c>
-      <c r="H94" t="str">
+      <c r="I94" t="str">
         <v>$ 43,091.00</v>
       </c>
-      <c r="I94" t="str">
+      <c r="J94" t="str">
         <v>$ 44,705.00</v>
       </c>
     </row>
@@ -3139,24 +3421,27 @@
         <v>2024</v>
       </c>
       <c r="C95" t="str">
-        <v>M4242:CARNIVAL EX AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D95" t="str">
+        <v>EX AUTO</v>
+      </c>
+      <c r="E95" t="str">
         <v>D2U: BLUE(D2U)</v>
       </c>
-      <c r="E95" t="str">
+      <c r="F95" t="str">
         <v>GYT: GRAY(GYT)</v>
       </c>
-      <c r="F95" t="str">
+      <c r="G95" t="str">
         <v>010</v>
       </c>
-      <c r="G95" t="str">
+      <c r="H95" t="str">
         <v>CA CF8 CN STD</v>
       </c>
-      <c r="H95" t="str">
+      <c r="I95" t="str">
         <v>$ 39,865.00</v>
       </c>
-      <c r="I95" t="str">
+      <c r="J95" t="str">
         <v>$ 40,935.00</v>
       </c>
     </row>
@@ -3168,24 +3453,27 @@
         <v>2024</v>
       </c>
       <c r="C96" t="str">
-        <v>M4232:CARNIVAL LX SEAT PACKAGE AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D96" t="str">
+        <v>LX SEAT PACKAGE AUTO</v>
+      </c>
+      <c r="E96" t="str">
         <v>ABP: BLACK(ABP)</v>
       </c>
-      <c r="E96" t="str">
+      <c r="F96" t="str">
         <v>GYT: GRAY(GYT)</v>
       </c>
-      <c r="F96" t="str">
+      <c r="G96" t="str">
         <v>010</v>
       </c>
-      <c r="G96" t="str">
+      <c r="H96" t="str">
         <v>CA CF8 STD</v>
       </c>
-      <c r="H96" t="str">
+      <c r="I96" t="str">
         <v>$ 36,406.00</v>
       </c>
-      <c r="I96" t="str">
+      <c r="J96" t="str">
         <v>$ 37,380.00</v>
       </c>
     </row>
@@ -3197,31 +3485,34 @@
         <v>2024</v>
       </c>
       <c r="C97" t="str">
-        <v>M4232:CARNIVAL LX SEAT PACKAGE AUTO</v>
+        <v>CARNIVAL</v>
       </c>
       <c r="D97" t="str">
+        <v>LX SEAT PACKAGE AUTO</v>
+      </c>
+      <c r="E97" t="str">
         <v>C7R: RED(C7R)</v>
       </c>
-      <c r="E97" t="str">
+      <c r="F97" t="str">
         <v>JY2: BROWN(JY2)</v>
       </c>
-      <c r="F97" t="str">
+      <c r="G97" t="str">
         <v>010</v>
       </c>
-      <c r="G97" t="str">
+      <c r="H97" t="str">
         <v>CF8 STD WL</v>
       </c>
-      <c r="H97" t="str">
+      <c r="I97" t="str">
         <v>$ 35,919.00</v>
       </c>
-      <c r="I97" t="str">
+      <c r="J97" t="str">
         <v>$ 36,855.00</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I97"/>
+  <autoFilter ref="A1:J97"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I97"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J97"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>